<commit_message>
adjusted script to read cols A and B, dictionary instead of List of dictionaries
</commit_message>
<xml_diff>
--- a/testfiles/en-SV.xlsx
+++ b/testfiles/en-SV.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oelll\Dropbox\_ME\III Professionella Expertis\C# Project\_EXCEL_ExcelAllLanguagesCommonDenominator\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernd\Downloads\Csharp\_EXCEL_ExcelAllLanguagesCommonDenominator\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89805714-41D5-41EE-B7CF-57BD983059EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A2F792-434F-4FDA-96E3-61DECAB73400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="23715" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -45,12 +45,6 @@
     <t>Signalförbättring</t>
   </si>
   <si>
-    <t>Ich go to the cinema every Thursday.</t>
-  </si>
-  <si>
-    <t>Jag gå på bio varje Tursdag.</t>
-  </si>
-  <si>
     <t>Who are you?</t>
   </si>
   <si>
@@ -70,6 +64,12 @@
   </si>
   <si>
     <t>(the next empty column).</t>
+  </si>
+  <si>
+    <t>I go to the cinema every Thursday.</t>
+  </si>
+  <si>
+    <t>Jag gå på bio varje Torsdag.</t>
   </si>
 </sst>
 </file>
@@ -133,7 +133,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,10 +414,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
@@ -432,18 +432,18 @@
         <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -454,18 +454,18 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>